<commit_message>
data for chub presence absence combined, model attempted
</commit_message>
<xml_diff>
--- a/tables/Example_node_flow_needs.xlsx
+++ b/tables/Example_node_flow_needs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katieirving/Documents/git/SOC_tier_3/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67EB519-D628-094A-B874-4B23284E25CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F58E34-9D88-094D-8BB5-BC5CE727AADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2860" windowWidth="27240" windowHeight="16440" xr2:uid="{9E3D7737-002B-7A4A-AF09-ABC2A729461C}"/>
+    <workbookView xWindow="-31380" yWindow="1840" windowWidth="27240" windowHeight="16440" xr2:uid="{9E3D7737-002B-7A4A-AF09-ABC2A729461C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="51">
   <si>
     <t>Species</t>
   </si>
@@ -130,6 +130,63 @@
   </si>
   <si>
     <t>&lt;0.4</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>&lt;5cm</t>
+  </si>
+  <si>
+    <t>&lt;4000 W/sqm</t>
+  </si>
+  <si>
+    <t>&lt;30 cm</t>
+  </si>
+  <si>
+    <t>&lt;0.4 m/s</t>
+  </si>
+  <si>
+    <t>&lt;15 cm</t>
+  </si>
+  <si>
+    <t>&lt;0.05 m/s</t>
+  </si>
+  <si>
+    <t>30-65 cm</t>
+  </si>
+  <si>
+    <t>35-60</t>
+  </si>
+  <si>
+    <t>&lt;0.8</t>
+  </si>
+  <si>
+    <t>&lt;0.7</t>
+  </si>
+  <si>
+    <t>&gt;5cm</t>
+  </si>
+  <si>
+    <t>&lt;28 cm</t>
+  </si>
+  <si>
+    <t>&lt;22 Pa</t>
+  </si>
+  <si>
+    <t>&lt;22</t>
+  </si>
+  <si>
+    <t>&lt;24</t>
+  </si>
+  <si>
+    <t>&lt;14</t>
+  </si>
+  <si>
+    <t>&lt;18</t>
+  </si>
+  <si>
+    <t>&lt;0.5 (Pa)</t>
   </si>
 </sst>
 </file>
@@ -171,9 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,20 +546,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6EBC7E2-41C4-A349-A104-11AFB7699DBC}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D19" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,10 +574,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -529,16 +591,19 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -549,16 +614,19 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -575,10 +643,13 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -595,10 +666,13 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -615,10 +689,13 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -635,10 +712,13 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -655,10 +735,13 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -675,10 +758,13 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -695,10 +781,13 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -715,10 +804,13 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -731,11 +823,11 @@
       <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -746,16 +838,19 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -766,16 +861,19 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -791,11 +889,14 @@
       <c r="E17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -811,11 +912,14 @@
       <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -831,11 +935,14 @@
       <c r="E19" t="s">
         <v>18</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -851,11 +958,14 @@
       <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -871,11 +981,14 @@
       <c r="E21" t="s">
         <v>17</v>
       </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -891,11 +1004,14 @@
       <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -911,11 +1027,14 @@
       <c r="E23" t="s">
         <v>17</v>
       </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -931,7 +1050,10 @@
       <c r="E24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>